<commit_message>
updated extract_json to correctly add finished levels to started levels
</commit_message>
<xml_diff>
--- a/generators/logs.xlsx
+++ b/generators/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,255 +463,255 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Level {"level":3,"type":"Moves","xDim":8,"yDim":8,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":12,"obstacleTypes":["Blue","Yellow"]}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-01-24T18:02:03.325</t>
+          <t>2024-02-06T18:50:50.989</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Shuffle</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Shuffle No more moves</t>
+          <t>Level {"level":6,"type":"Colors","xDim":6,"yDim":7,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":13,"obstacleTypes":["Blue","Green","Pink"]}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-01-24T18:02:21.726</t>
+          <t>2024-02-06T18:52:32.964</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":9,"type":"Timer","xDim":6,"yDim":6,"numMoves":30,"score1":3000,"score2":3500,"score3":4000,"targetScore":4000,"timeInSeconds":80,"numOfObstacles":7,"obstacleTypes":["Pink","Red","Purple"]}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-01-24T18:53:58.702</t>
+          <t>2024-02-06T18:54:56.472</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-01-24T18:54:23.753</t>
+          <t>2024-02-06T18:55:21.480</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":13,"type":"Timer","xDim":9,"yDim":7,"numMoves":35,"score1":4000,"score2":4500,"score3":5000,"targetScore":5000,"timeInSeconds":90,"numOfObstacles":12,"obstacleTypes":["Blue","Red"]}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-01-24T18:54:26.666</t>
+          <t>2024-02-07T18:28:02.267</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":16,"type":"Obstacle","xDim":6,"yDim":6,"numMoves":35,"score1":4000,"score2":4500,"score3":5000,"targetScore":5000,"timeInSeconds":90,"numOfObstacles":7,"obstacleTypes":["Yellow","Pink","Purple","Red"]}</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-01-24T18:54:36.131</t>
+          <t>2024-02-08T17:32:10.535</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":19,"type":"Moves","xDim":9,"yDim":10,"numMoves":40,"score1":5000,"score2":5500,"score3":6000,"targetScore":6000,"timeInSeconds":100,"numOfObstacles":18,"obstacleTypes":["Yellow","Pink","Blue"]}</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-01-24T18:54:40.705</t>
+          <t>2024-02-08T17:34:47.427</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":25,"type":"Timer","xDim":10,"yDim":9,"numMoves":50,"score1":7000,"score2":7500,"score3":8000,"targetScore":8000,"timeInSeconds":120,"numOfObstacles":18,"obstacleTypes":["Yellow"]}</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-01-24T18:54:49.481</t>
+          <t>2024-02-09T17:58:40.920</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-06–18:46-5kE5d5J9bcqdKNe</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":28,"type":"Obstacle","xDim":9,"yDim":8,"numMoves":50,"score1":7000,"score2":7500,"score3":8000,"targetScore":8000,"timeInSeconds":120,"numOfObstacles":14,"obstacleTypes":["Green","Red","Yellow"]}</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-01-24T18:55:04.956</t>
+          <t>2024-02-09T18:02:42.693</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Safari/605.1.15</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -721,208 +721,208 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-01-24T18:55:13.153</t>
+          <t>2024-02-11T11:10:05.043</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":15,"type":"Moves","xDim":6,"yDim":8,"numMoves":35,"score1":4000,"score2":4500,"score3":5000,"targetScore":5000,"timeInSeconds":90,"numOfObstacles":9,"obstacleTypes":["Purple","Blue","Green"]}</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-01-24T18:55:45.749</t>
+          <t>2024-02-11T11:31:43.277</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":22,"type":"Colors","xDim":9,"yDim":9,"numMoves":45,"score1":6000,"score2":6500,"score3":7000,"targetScore":7000,"timeInSeconds":110,"numOfObstacles":19,"obstacleTypes":["Yellow","Purple","Blue"]}</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-01-24T18:56:22.829</t>
+          <t>2024-02-14T07:01:50.420</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-01-24T18:56:40.247</t>
+          <t>2024-02-14T07:08:23.225</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-01-24T18:57:43.604</t>
+          <t>2024-02-14T07:11:03.357</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":28,"type":"Obstacle","xDim":9,"yDim":8,"numMoves":50,"score1":7000,"score2":7500,"score3":8000,"targetScore":8000,"timeInSeconds":120,"numOfObstacles":14,"obstacleTypes":["Green","Red","Yellow"]}</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-01-24T18:58:31.913</t>
+          <t>2024-02-14T14:13:11.584</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":28,"type":"Obstacle","xDim":9,"yDim":8,"numMoves":50,"score1":7000,"score2":7500,"score3":8000,"targetScore":8000,"timeInSeconds":120,"numOfObstacles":14,"obstacleTypes":["Green","Red","Yellow"]}</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-01-26T12:11:19.959</t>
+          <t>2024-02-14T19:41:45.702</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-01-26T12:11:30.095</t>
+          <t>2024-02-16T12:48:54.208</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -937,46 +937,46 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-01-26T12:11:31.298</t>
+          <t>2024-02-16T14:40:43.038</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Level {"level":24,"type":"Obstacle","xDim":10,"yDim":10,"numMoves":45,"score1":6000,"score2":6500,"score3":7000,"targetScore":7000,"timeInSeconds":110,"numOfObstacles":20,"obstacleTypes":["Green"]}</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-01-26T12:11:41.727</t>
+          <t>2024-02-16T14:40:36.324</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -991,397 +991,397 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-01-26T12:13:12.178</t>
+          <t>2024-02-16T14:42:11.422</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>V03-24-02-09–10:10-0Z8tTc5mAWYJk15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-01-26T12:13:48.260</t>
+          <t>2024-02-16T14:45:36.092</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2024-01-26T12:13:48.974</t>
+          <t>2024-02-16T14:01:40.215</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":2,"type":"Colors","xDim":8,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":14,"obstacleTypes":["Purple","Red","Pink","Blue"]}</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-01-26T12:14:02.064</t>
+          <t>2024-02-16T16:24:41.955</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Level {"level":3,"type":"Moves","xDim":8,"yDim":8,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":12,"obstacleTypes":["Blue","Yellow"]}</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2024-01-26T12:14:32.919</t>
+          <t>2024-02-16T16:25:35.410</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2024-01-27T15:54:14.869</t>
+          <t>2024-02-16T16:26:15.268</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Level {"level":4,"type":"Obstacle","xDim":7,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":8,"obstacleTypes":["Purple","Green"]}</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2024-01-29T18:14:14.951</t>
+          <t>2024-02-16T16:26:08.437</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Level {"level":5,"type":"Timer","xDim":8,"yDim":9,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":14,"obstacleTypes":["Green","Blue"]}</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2024-01-29T18:14:45.091</t>
+          <t>2024-02-16T16:27:32.925</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-18–19:18-q7IQ4iJK6blvaoG</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Level {"level":7,"type":"Moves","xDim":8,"yDim":9,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":14,"obstacleTypes":["Red"]}</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2024-01-26T14:42:09.088</t>
+          <t>2024-02-16T18:24:28.025</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-19–12:08-H6FwYapNk5I8Tp5</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":9,"type":"Timer","xDim":6,"yDim":6,"numMoves":30,"score1":3000,"score2":3500,"score3":4000,"targetScore":4000,"timeInSeconds":80,"numOfObstacles":7,"obstacleTypes":["Pink","Red","Purple"]}</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2024-01-25T05:01:45.681</t>
+          <t>2024-02-17T04:26:58.104</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-19–12:59-DeitIN4PGCSqjO3</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2024-01-26T18:26:48.277</t>
+          <t>2024-02-17T04:27:22.106</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-19–12:59-DeitIN4PGCSqjO3</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":11,"type":"Moves","xDim":9,"yDim":8,"numMoves":30,"score1":3000,"score2":3500,"score3":4000,"targetScore":4000,"timeInSeconds":80,"numOfObstacles":14,"obstacleTypes":["Yellow"]}</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2024-01-26T18:27:20.510</t>
+          <t>2024-02-17T06:29:05.370</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-23–20:48-d2R10YCryURYw5M</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Level {"level":12,"type":"Obstacle","xDim":8,"yDim":6,"numMoves":30,"score1":3000,"score2":3500,"score3":4000,"targetScore":4000,"timeInSeconds":80,"numOfObstacles":9,"obstacleTypes":["Purple","Green","Pink"]}</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2024-01-24T17:33:05.812</t>
+          <t>2024-02-17T06:30:20.750</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-23–20:48-d2R10YCryURYw5M</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Level {"level":13,"type":"Timer","xDim":9,"yDim":7,"numMoves":35,"score1":4000,"score2":4500,"score3":5000,"targetScore":5000,"timeInSeconds":90,"numOfObstacles":12,"obstacleTypes":["Blue","Red"]}</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2024-01-24T17:33:34.105</t>
+          <t>2024-02-17T06:31:08.710</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–16:22-01YJAZTvKK43LdE</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Level {"level":15,"type":"Moves","xDim":6,"yDim":8,"numMoves":35,"score1":4000,"score2":4500,"score3":5000,"targetScore":5000,"timeInSeconds":90,"numOfObstacles":9,"obstacleTypes":["Purple","Blue","Green"]}</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2024-01-24T17:32:46.617</t>
+          <t>2024-02-17T10:12:13.721</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–16:35-LpLo97rscJMsfX7</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1396,1558 +1396,1558 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2024-01-24T17:32:53.737</t>
+          <t>2024-02-16T16:51:20.572</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–16:35-LpLo97rscJMsfX7</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2024-01-24T17:33:02.898</t>
+          <t>2024-02-16T18:54:43.231</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2024-01-24T17:34:40.385</t>
+          <t>2024-02-16T17:22:16.838</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2024-01-24T17:34:48.324</t>
+          <t>2024-02-16T17:24:29.223</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2024-01-24T17:34:57.895</t>
+          <t>2024-02-16T17:25:32.869</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2024-01-24T17:35:25.168</t>
+          <t>2024-02-16T17:35:58.150</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K3'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2024-01-24T17:35:33.061</t>
+          <t>2024-02-16T17:59:32.073</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":31,"type":"Moves","xDim":6,"yDim":8,"numMoves":55,"score1":8000,"score2":8500,"score3":9000,"targetScore":9000,"timeInSeconds":130,"numOfObstacles":9,"obstacleTypes":["Blue"]}</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2024-01-25T14:04:22.145</t>
+          <t>2024-02-16T18:01:56.140</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2024-01-25T14:04:29.796</t>
+          <t>2024-02-16T18:03:28.850</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2024-01-25T14:04:37.916</t>
+          <t>2024-02-16T18:05:11.500</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:04-5TldOaCAycjwHpv</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":39,"type":"Moves","xDim":7,"yDim":8,"numMoves":65,"score1":10000,"score2":10500,"score3":11000,"targetScore":11000,"timeInSeconds":150,"numOfObstacles":11,"obstacleTypes":["Red","Yellow","Pink","Blue"]}</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2024-01-25T14:04:45.551</t>
+          <t>2024-02-17T06:02:12.324</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:05-zbE8VQByDwBedDn</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2024-01-25T14:04:53.018</t>
+          <t>2024-02-16T17:20:47.293</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 14; SAMSUNG SM-G991B) AppleWebKit/537.36 (KHTML, like Gecko) SamsungBrowser/23.0 Chrome/115.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:05-zbE8VQByDwBedDn</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":20,"type":"Obstacle","xDim":9,"yDim":7,"numMoves":40,"score1":5000,"score2":5500,"score3":6000,"targetScore":6000,"timeInSeconds":100,"numOfObstacles":12,"obstacleTypes":["Green","Yellow","Blue"]}</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2024-01-25T14:05:03.661</t>
+          <t>2024-02-16T17:52:49.356</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 14; SAMSUNG SM-G991B) AppleWebKit/537.36 (KHTML, like Gecko) SamsungBrowser/23.0 Chrome/115.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–17:05-zbE8VQByDwBedDn</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2024-01-25T14:05:12.630</t>
+          <t>2024-02-16T17:54:05.405</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 14; SAMSUNG SM-G991B) AppleWebKit/537.36 (KHTML, like Gecko) SamsungBrowser/23.0 Chrome/115.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–18:36-CaibBsnLVP3oh6h</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2024-01-25T14:05:21.148</t>
+          <t>2024-02-16T18:38:33.925</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–18:36-CaibBsnLVP3oh6h</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":2,"type":"Colors","xDim":8,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":14,"obstacleTypes":["Purple","Red","Pink","Blue"]}</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2024-01-25T14:05:40.268</t>
+          <t>2024-02-16T18:40:20.504</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–18:36-CaibBsnLVP3oh6h</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":4,"type":"Obstacle","xDim":7,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":8,"obstacleTypes":["Purple","Green"]}</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2024-01-25T14:05:48.153</t>
+          <t>2024-02-16T18:42:33.636</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–18:36-CaibBsnLVP3oh6h</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2024-01-25T14:05:56.321</t>
+          <t>2024-02-17T05:53:30.282</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–18:36-CaibBsnLVP3oh6h</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":4,"type":"Obstacle","xDim":7,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":8,"obstacleTypes":["Purple","Green"]}</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2024-01-25T14:06:17.629</t>
+          <t>2024-02-17T05:55:43.166</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-16–18:36-CaibBsnLVP3oh6h</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":6,"type":"Colors","xDim":6,"yDim":7,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":13,"obstacleTypes":["Blue","Green","Pink"]}</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2024-01-25T14:06:31.448</t>
+          <t>2024-02-17T05:59:23.216</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-17–10:16-8cklHOIuSKDpYAn</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":3,"type":"Moves","xDim":8,"yDim":8,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":12,"obstacleTypes":["Blue","Yellow"]}</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2024-01-25T14:06:39.984</t>
+          <t>2024-02-17T10:21:39.602</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_0_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.0.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–16:02-Ki9i1U8HCQK09Fd</t>
+          <t>flutter-V04-24-02-17–10:16-8cklHOIuSKDpYAn</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>closeFAB</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Level {"level":5,"type":"Timer","xDim":8,"yDim":9,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":14,"obstacleTypes":["Green","Blue"]}</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2024-01-25T14:06:47.719</t>
+          <t>2024-02-17T10:27:08.663</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_0_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.0.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–17:30-cMcahqsoQ8zm99M</t>
+          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2024-01-24T17:30:46.292</t>
+          <t>2024-02-05T17:26:57.566</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–17:30-cMcahqsoQ8zm99M</t>
+          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2024-01-24T17:31:28.958</t>
+          <t>2024-02-05T17:29:48.999</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–17:30-cMcahqsoQ8zm99M</t>
+          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level {"level":30,"type":"Colors","xDim":9,"yDim":8,"numMoves":55,"score1":8000,"score2":8500,"score3":9000,"targetScore":9000,"timeInSeconds":130,"numOfObstacles":26,"obstacleTypes":["Red","Yellow","Purple","Blue"]}</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2024-01-24T17:31:51.479</t>
+          <t>2024-02-05T21:51:56.849</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–17:30-cMcahqsoQ8zm99M</t>
+          <t>testVersion-V02-24-01-18–14:53-GIyhuiNMa5KNsMp</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2024-01-24T17:32:30.611</t>
+          <t>2024-02-07T00:19:56.122</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–17:30-cMcahqsoQ8zm99M</t>
+          <t>testVersion-V02-24-02-03–16:40-cCVmNbabskJtvqV</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2024-01-24T17:32:53.483</t>
+          <t>2024-02-05T20:21:49.179</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–17:30-cMcahqsoQ8zm99M</t>
+          <t>testVersion-V02-24-02-03–16:40-cCVmNbabskJtvqV</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Shuffle</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Shuffle No more moves</t>
+          <t>Level {"level":5,"type":"Timer","xDim":8,"yDim":9,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":14,"obstacleTypes":["Green","Blue"]}</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2024-01-24T17:33:29.301</t>
+          <t>2024-02-05T20:50:22.050</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:10-lQhylEVtncdtzCJ</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level 0</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2024-01-24T18:11:38.755</t>
+          <t>2024-02-05T17:19:14.867</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:12-ypxdYfEhFY0wTtg</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2024-01-24T18:13:01.980</t>
+          <t>2024-02-05T17:27:30.862</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:14-iF7IgMruK7gvmpc</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2024-01-24T18:14:06.013</t>
+          <t>2024-02-05T17:27:43.037</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:16-HTQvPDOkO49OlUX</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level 0</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2024-01-24T18:16:49.769</t>
+          <t>2024-02-05T17:30:59.098</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:18-D2PPzXI32fhtj1D</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2024-01-24T18:18:26.547</t>
+          <t>2024-02-05T17:31:23.327</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:19-QEcJwaRnguBytis</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2024-01-24T18:19:36.266</t>
+          <t>2024-02-05T17:34:13.950</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:19-QEcJwaRnguBytis</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2024-01-24T18:21:19.292</t>
+          <t>2024-02-06T15:20:35.621</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:19-QEcJwaRnguBytis</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level {"level":16,"type":"Obstacle","xDim":6,"yDim":6,"numMoves":35,"score1":4000,"score2":4500,"score3":5000,"targetScore":5000,"timeInSeconds":90,"numOfObstacles":7,"obstacleTypes":["Yellow","Pink","Purple","Red"]}</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2024-01-24T18:21:43.977</t>
+          <t>2024-02-06T15:32:12.359</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:22-2H7csOnBDMga90U</t>
+          <t>testVersion-V02-24-02-05–17:07-dKYEy72Q5S5EQXX</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2024-01-24T18:25:02.283</t>
+          <t>2024-02-06T15:32:25.844</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:22-2H7csOnBDMga90U</t>
+          <t>testVersion-V03-24-02-07–17:17-jXtN1aC69F8CY6D</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2024-01-24T18:25:23.503</t>
+          <t>2024-02-07T17:17:44.252</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:26-iPvGlP4lkHeThxN</t>
+          <t>testVersion-V03-24-02-07–17:17-jXtN1aC69F8CY6D</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2024-01-24T18:26:50.032</t>
+          <t>2024-02-07T17:18:01.023</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:30-XKus7ZSpHDRFPNl</t>
+          <t>testVersion-V03-24-02-07–17:17-jXtN1aC69F8CY6D</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2024-01-24T18:30:26.473</t>
+          <t>2024-02-07T17:20:30.722</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:32-aMA9lRp8Llsn8aU</t>
+          <t>testVersion-V03-24-02-07–17:17-jXtN1aC69F8CY6D</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2024-01-24T18:32:34.501</t>
+          <t>2024-02-14T09:48:56.424</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:32-aMA9lRp8Llsn8aU</t>
+          <t>testVersion-V03-24-02-07–17:17-jXtN1aC69F8CY6D</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>onUnitySceneLoaded</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Unity not ready</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2024-01-24T18:32:39.114</t>
+          <t>2024-02-14T09:50:12.600</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:32-aMA9lRp8Llsn8aU</t>
+          <t>testVersion-V03-24-02-07–17:24-RJbk6oMDjJqLBrZ</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>onUnitySceneLoaded</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Unity not ready</t>
+          <t>Level {"level":2,"type":"Colors","xDim":8,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":14,"obstacleTypes":["Purple","Red","Pink","Blue"]}</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2024-01-24T18:32:39.115</t>
+          <t>2024-02-10T14:04:03.636</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:32-aMA9lRp8Llsn8aU</t>
+          <t>testVersion-V03-24-02-07–17:24-RJbk6oMDjJqLBrZ</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level {"level":3,"type":"Moves","xDim":8,"yDim":8,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":12,"obstacleTypes":["Blue","Yellow"]}</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2024-01-24T18:33:36.296</t>
+          <t>2024-02-10T14:04:36.916</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:40-ZAYRpWWifQqAkOn</t>
+          <t>testVersion-V03-24-02-07–17:24-RJbk6oMDjJqLBrZ</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level {"level":4,"type":"Obstacle","xDim":7,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":8,"obstacleTypes":["Purple","Green"]}</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2024-01-24T18:40:20.141</t>
+          <t>2024-02-10T14:05:24.020</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:40-ZAYRpWWifQqAkOn</t>
+          <t>testVersion-V03-24-02-07–17:24-RJbk6oMDjJqLBrZ</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2024-01-24T18:41:59.240</t>
+          <t>2024-02-10T14:05:39.684</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:44-f1IU7hFgyM3THqN</t>
+          <t>testVersion-V03-24-02-07–17:24-RJbk6oMDjJqLBrZ</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Level {"level":5,"type":"Timer","xDim":8,"yDim":9,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":14,"obstacleTypes":["Green","Blue"]}</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2024-01-24T18:44:33.771</t>
+          <t>2024-02-10T14:06:36.506</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_4 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:44-f1IU7hFgyM3THqN</t>
+          <t>testVersion-V03-24-02-08–18:05-aPWM8K2j9MXNu8E</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2024-01-24T18:45:19.549</t>
+          <t>2024-02-08T18:08:06.143</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:44-f1IU7hFgyM3THqN</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2024-01-24T18:45:21.533</t>
+          <t>2024-02-09T08:51:41.715</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:44-f1IU7hFgyM3THqN</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2024-01-24T18:45:28.323</t>
+          <t>2024-02-09T08:51:42.481</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-24–18:44-f1IU7hFgyM3THqN</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Instance of 'WebUnityWidgetController'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2024-01-24T18:45:30.423</t>
+          <t>2024-02-09T08:51:43.097</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2024-01-25T13:49:58.557</t>
+          <t>2024-02-09T08:53:18.458</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2024-01-25T13:50:36.181</t>
+          <t>2024-02-09T08:53:19.207</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2024-01-25T13:52:47.213</t>
+          <t>2024-02-09T08:55:06.064</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2024-01-25T13:53:31.485</t>
+          <t>2024-02-09T08:55:42.324</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:09.308</t>
+          <t>2024-02-09T08:55:43.406</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Level {"level":4,"type":"Obstacle","xDim":7,"yDim":6,"numMoves":20,"score1":1000,"score2":1500,"score3":2000,"targetScore":2000,"timeInSeconds":60,"numOfObstacles":8,"obstacleTypes":["Purple","Green"]}</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:27.952</t>
+          <t>2024-02-09T08:56:26.206</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:47-hCJ9DrrzcaqCnk0</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>onUnityCreated</t>
+          <t>musicFab</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Instance of 'minified:K4'</t>
+          <t>Music FAB pressed</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2024-01-25T13:56:22.515</t>
+          <t>2024-02-09T08:56:37.844</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Safari/605.1.15</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2962,19 +2962,19 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:36.268</t>
+          <t>2024-02-09T08:56:38.859</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2989,19 +2989,19 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:36.772</t>
+          <t>2024-02-09T08:58:27.689</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3016,46 +3016,46 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:37.236</t>
+          <t>2024-02-09T08:58:28.387</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>RestartGame</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Level {"level":7,"type":"Moves","xDim":8,"yDim":9,"numMoves":25,"score1":2000,"score2":2500,"score3":3000,"targetScore":3000,"timeInSeconds":70,"numOfObstacles":14,"obstacleTypes":["Red"]}</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:37.452</t>
+          <t>2024-02-09T09:00:48.521</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3070,19 +3070,19 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:37.667</t>
+          <t>2024-02-09T09:00:57.704</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3097,19 +3097,19 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:37.842</t>
+          <t>2024-02-09T09:00:58.652</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3124,19 +3124,19 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:38.002</t>
+          <t>2024-02-09T09:01:51.753</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3151,19 +3151,19 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:38.145</t>
+          <t>2024-02-09T09:01:53.251</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3178,19 +3178,19 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:38.301</t>
+          <t>2024-02-09T09:03:23.149</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3205,127 +3205,127 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:38.429</t>
+          <t>2024-02-09T09:03:24.298</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-09–08:45-QKg5phRFXyCKJee</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:38.977</t>
+          <t>2024-02-09T09:06:18.290</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-13–10:36-maJBXcgXhtHVv9e</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>closeFAB</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Close FAB pressed</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:39.132</t>
+          <t>2024-02-13T10:37:09.356</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-13–12:51-VZEruV9oR9S0cEG</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>musicFab</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Music FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:39.441</t>
+          <t>2024-02-13T12:51:51.818</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:54-HGJqLFVSJjxlfIy</t>
+          <t>testVersion-V03-24-02-13–12:51-VZEruV9oR9S0cEG</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>closeFABError</t>
+          <t>Shuffle</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Close FAB pressed</t>
+          <t>Shuffle No more moves</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2024-01-25T13:54:40.419</t>
+          <t>2024-02-13T12:52:01.617</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
+          <t>testVersion-V03-24-02-16–16:53-ph75aJaJROK2jSa</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3340,19 +3340,19 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:51.284</t>
+          <t>2024-02-16T16:54:01.856</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
+          <t>testVersion-V03-24-02-16–16:53-ph75aJaJROK2jSa</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3367,19 +3367,19 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:51.964</t>
+          <t>2024-02-16T16:54:06.146</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
+          <t>testVersion-V03-24-02-16–16:53-ph75aJaJROK2jSa</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3394,19 +3394,19 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:52.293</t>
+          <t>2024-02-16T16:54:07.262</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
+          <t>testVersion-V03-24-02-16–16:53-ph75aJaJROK2jSa</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3421,19 +3421,19 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:52.445</t>
+          <t>2024-02-16T16:54:32.338</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
+          <t>testVersion-V03-24-02-16–16:53-ph75aJaJROK2jSa</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3448,19 +3448,19 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:52.615</t>
+          <t>2024-02-16T16:54:34.851</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
+          <t>testVersion-V03-24-02-16–16:53-ph75aJaJROK2jSa</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3475,1011 +3475,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2024-01-25T13:55:52.788</t>
+          <t>2024-02-16T16:55:40.519</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:55:53.315</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:55:53.479</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:55:53.656</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:55:54.253</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:55:54.400</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>closeFABError</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:55:54.973</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–13:55-zG61WLFECqKVuiR</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>2024-01-25T13:56:26.620</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-25–14:09-DfmWkxBcYZG30bp</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Shuffle</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Shuffle No more moves</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>2024-01-25T14:12:03.505</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 6.0; Nexus 5 Build/MRA58N) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:13-uyKYj83pVMQcQKc</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:13:59.340</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:16-WOwcL7noFki5wIo</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:17:13.131</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 13; SM-G981B) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/116.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:52-dNXs0t1VmpoI7d4</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:52:20.967</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:52-dNXs0t1VmpoI7d4</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:52:56.658</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:52-dNXs0t1VmpoI7d4</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:53:01.274</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:54-4BRNlw411QkaBAo</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:54:58.076</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:54-4BRNlw411QkaBAo</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:55:03.524</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:54-4BRNlw411QkaBAo</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:55:04.530</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:54-4BRNlw411QkaBAo</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:55:23.475</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–11:54-4BRNlw411QkaBAo</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>2024-01-26T11:55:36.881</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–12:02-blMbyqs2X6nOm8U</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>2024-01-26T12:02:23.427</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–12:05-45N8iabNICSq5Di</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>2024-01-26T12:05:28.956</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:04-PxvYfjjsDRttEoT</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:04:21.321</t>
-        </is>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:14-9qyO7bJ85Kvi8Qm</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:17:24.671</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:14-9qyO7bJ85Kvi8Qm</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:17:48.317</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:14-9qyO7bJ85Kvi8Qm</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:17:52.193</t>
-        </is>
-      </c>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:14-9qyO7bJ85Kvi8Qm</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:17:55.316</t>
-        </is>
-      </c>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:14-9qyO7bJ85Kvi8Qm</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:17:58.815</t>
-        </is>
-      </c>
-      <c r="E139" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–18:14-9qyO7bJ85Kvi8Qm</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>musicFab</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>Music FAB pressed</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>2024-01-26T18:17:58.847</t>
-        </is>
-      </c>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Shuffle</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Shuffle No more moves</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:02:59.662</t>
-        </is>
-      </c>
-      <c r="E141" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:05:06.228</t>
-        </is>
-      </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:05:17.639</t>
-        </is>
-      </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:05:24.823</t>
-        </is>
-      </c>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:05:43.394</t>
-        </is>
-      </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:05:50.262</t>
-        </is>
-      </c>
-      <c r="E146" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:05:57.830</t>
-        </is>
-      </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:06:15.841</t>
-        </is>
-      </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:06:23.277</t>
-        </is>
-      </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>testVersion-V02-24-01-26–22:01-7RxZZmIPyzbEMiV</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>closeFAB</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>Close FAB pressed</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>2024-01-26T22:06:31.645</t>
-        </is>
-      </c>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
     </row>

</xml_diff>